<commit_message>
Ajout de 2 sites web de pref
</commit_message>
<xml_diff>
--- a/Data/AFNIC-gouvfr-201907.xlsx
+++ b/Data/AFNIC-gouvfr-201907.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27940" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13960" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LISTE des sites web OFF" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7995" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7991" uniqueCount="1045">
   <si>
     <t>abonnement-presse.gouv.fr</t>
   </si>
@@ -3155,6 +3155,9 @@
   </si>
   <si>
     <t>NDD non intégré</t>
+  </si>
+  <si>
+    <t>Redirection</t>
   </si>
 </sst>
 </file>
@@ -3203,8 +3206,58 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="527">
+  <cellStyleXfs count="577">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3736,7 +3789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="527">
+  <cellStyles count="577">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -4000,6 +4053,31 @@
     <cellStyle name="Lien hypertexte" xfId="521" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="523" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="525" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="527" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="529" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="531" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="533" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="535" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="537" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="539" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="575" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -4263,6 +4341,31 @@
     <cellStyle name="Lien hypertexte visité" xfId="522" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="524" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="526" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="528" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="530" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="532" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="534" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="536" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="538" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="540" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="576" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -4603,10 +4706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B626"/>
+  <dimension ref="A1:B624"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A459" workbookViewId="0">
+      <selection activeCell="A485" sqref="A485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5180,7 +5283,7 @@
         <v>123</v>
       </c>
       <c r="B71" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -5188,7 +5291,7 @@
         <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -7513,7 +7616,7 @@
     </row>
     <row r="363" spans="1:2">
       <c r="A363" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="B363" t="s">
         <v>1041</v>
@@ -7521,7 +7624,7 @@
     </row>
     <row r="364" spans="1:2">
       <c r="A364" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="B364" t="s">
         <v>1041</v>
@@ -7529,7 +7632,7 @@
     </row>
     <row r="365" spans="1:2">
       <c r="A365" t="s">
-        <v>638</v>
+        <v>640</v>
       </c>
       <c r="B365" t="s">
         <v>1041</v>
@@ -7537,7 +7640,7 @@
     </row>
     <row r="366" spans="1:2">
       <c r="A366" t="s">
-        <v>639</v>
+        <v>641</v>
       </c>
       <c r="B366" t="s">
         <v>1041</v>
@@ -7545,7 +7648,7 @@
     </row>
     <row r="367" spans="1:2">
       <c r="A367" t="s">
-        <v>640</v>
+        <v>642</v>
       </c>
       <c r="B367" t="s">
         <v>1041</v>
@@ -7553,7 +7656,7 @@
     </row>
     <row r="368" spans="1:2">
       <c r="A368" t="s">
-        <v>641</v>
+        <v>643</v>
       </c>
       <c r="B368" t="s">
         <v>1041</v>
@@ -7561,7 +7664,7 @@
     </row>
     <row r="369" spans="1:2">
       <c r="A369" t="s">
-        <v>642</v>
+        <v>649</v>
       </c>
       <c r="B369" t="s">
         <v>1041</v>
@@ -7569,7 +7672,7 @@
     </row>
     <row r="370" spans="1:2">
       <c r="A370" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="B370" t="s">
         <v>1041</v>
@@ -7577,7 +7680,7 @@
     </row>
     <row r="371" spans="1:2">
       <c r="A371" t="s">
-        <v>649</v>
+        <v>651</v>
       </c>
       <c r="B371" t="s">
         <v>1041</v>
@@ -7585,7 +7688,7 @@
     </row>
     <row r="372" spans="1:2">
       <c r="A372" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B372" t="s">
         <v>1041</v>
@@ -7593,7 +7696,7 @@
     </row>
     <row r="373" spans="1:2">
       <c r="A373" t="s">
-        <v>651</v>
+        <v>653</v>
       </c>
       <c r="B373" t="s">
         <v>1041</v>
@@ -7601,7 +7704,7 @@
     </row>
     <row r="374" spans="1:2">
       <c r="A374" t="s">
-        <v>652</v>
+        <v>657</v>
       </c>
       <c r="B374" t="s">
         <v>1041</v>
@@ -7609,7 +7712,7 @@
     </row>
     <row r="375" spans="1:2">
       <c r="A375" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="B375" t="s">
         <v>1041</v>
@@ -7617,7 +7720,7 @@
     </row>
     <row r="376" spans="1:2">
       <c r="A376" t="s">
-        <v>657</v>
+        <v>659</v>
       </c>
       <c r="B376" t="s">
         <v>1041</v>
@@ -7625,7 +7728,7 @@
     </row>
     <row r="377" spans="1:2">
       <c r="A377" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B377" t="s">
         <v>1041</v>
@@ -7633,7 +7736,7 @@
     </row>
     <row r="378" spans="1:2">
       <c r="A378" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="B378" t="s">
         <v>1041</v>
@@ -7641,7 +7744,7 @@
     </row>
     <row r="379" spans="1:2">
       <c r="A379" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B379" t="s">
         <v>1041</v>
@@ -7649,7 +7752,7 @@
     </row>
     <row r="380" spans="1:2">
       <c r="A380" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B380" t="s">
         <v>1041</v>
@@ -7657,7 +7760,7 @@
     </row>
     <row r="381" spans="1:2">
       <c r="A381" t="s">
-        <v>663</v>
+        <v>667</v>
       </c>
       <c r="B381" t="s">
         <v>1041</v>
@@ -7665,7 +7768,7 @@
     </row>
     <row r="382" spans="1:2">
       <c r="A382" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="B382" t="s">
         <v>1041</v>
@@ -7673,7 +7776,7 @@
     </row>
     <row r="383" spans="1:2">
       <c r="A383" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
       <c r="B383" t="s">
         <v>1041</v>
@@ -7681,7 +7784,7 @@
     </row>
     <row r="384" spans="1:2">
       <c r="A384" t="s">
-        <v>668</v>
+        <v>677</v>
       </c>
       <c r="B384" t="s">
         <v>1041</v>
@@ -7689,7 +7792,7 @@
     </row>
     <row r="385" spans="1:2">
       <c r="A385" t="s">
-        <v>669</v>
+        <v>678</v>
       </c>
       <c r="B385" t="s">
         <v>1041</v>
@@ -7697,7 +7800,7 @@
     </row>
     <row r="386" spans="1:2">
       <c r="A386" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="B386" t="s">
         <v>1041</v>
@@ -7705,7 +7808,7 @@
     </row>
     <row r="387" spans="1:2">
       <c r="A387" t="s">
-        <v>678</v>
+        <v>683</v>
       </c>
       <c r="B387" t="s">
         <v>1041</v>
@@ -7713,7 +7816,7 @@
     </row>
     <row r="388" spans="1:2">
       <c r="A388" t="s">
-        <v>680</v>
+        <v>684</v>
       </c>
       <c r="B388" t="s">
         <v>1041</v>
@@ -7721,7 +7824,7 @@
     </row>
     <row r="389" spans="1:2">
       <c r="A389" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="B389" t="s">
         <v>1041</v>
@@ -7729,7 +7832,7 @@
     </row>
     <row r="390" spans="1:2">
       <c r="A390" t="s">
-        <v>684</v>
+        <v>688</v>
       </c>
       <c r="B390" t="s">
         <v>1041</v>
@@ -7737,7 +7840,7 @@
     </row>
     <row r="391" spans="1:2">
       <c r="A391" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="B391" t="s">
         <v>1041</v>
@@ -7745,7 +7848,7 @@
     </row>
     <row r="392" spans="1:2">
       <c r="A392" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B392" t="s">
         <v>1041</v>
@@ -7753,7 +7856,7 @@
     </row>
     <row r="393" spans="1:2">
       <c r="A393" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="B393" t="s">
         <v>1041</v>
@@ -7761,7 +7864,7 @@
     </row>
     <row r="394" spans="1:2">
       <c r="A394" t="s">
-        <v>690</v>
+        <v>698</v>
       </c>
       <c r="B394" t="s">
         <v>1041</v>
@@ -7769,7 +7872,7 @@
     </row>
     <row r="395" spans="1:2">
       <c r="A395" t="s">
-        <v>691</v>
+        <v>699</v>
       </c>
       <c r="B395" t="s">
         <v>1041</v>
@@ -7777,7 +7880,7 @@
     </row>
     <row r="396" spans="1:2">
       <c r="A396" t="s">
-        <v>698</v>
+        <v>702</v>
       </c>
       <c r="B396" t="s">
         <v>1041</v>
@@ -7785,7 +7888,7 @@
     </row>
     <row r="397" spans="1:2">
       <c r="A397" t="s">
-        <v>699</v>
+        <v>707</v>
       </c>
       <c r="B397" t="s">
         <v>1041</v>
@@ -7793,7 +7896,7 @@
     </row>
     <row r="398" spans="1:2">
       <c r="A398" t="s">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="B398" t="s">
         <v>1041</v>
@@ -7801,7 +7904,7 @@
     </row>
     <row r="399" spans="1:2">
       <c r="A399" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
       <c r="B399" t="s">
         <v>1041</v>
@@ -7809,7 +7912,7 @@
     </row>
     <row r="400" spans="1:2">
       <c r="A400" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="B400" t="s">
         <v>1041</v>
@@ -7817,7 +7920,7 @@
     </row>
     <row r="401" spans="1:2">
       <c r="A401" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="B401" t="s">
         <v>1041</v>
@@ -7825,7 +7928,7 @@
     </row>
     <row r="402" spans="1:2">
       <c r="A402" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="B402" t="s">
         <v>1041</v>
@@ -7833,7 +7936,7 @@
     </row>
     <row r="403" spans="1:2">
       <c r="A403" t="s">
-        <v>716</v>
+        <v>721</v>
       </c>
       <c r="B403" t="s">
         <v>1041</v>
@@ -7841,7 +7944,7 @@
     </row>
     <row r="404" spans="1:2">
       <c r="A404" t="s">
-        <v>717</v>
+        <v>722</v>
       </c>
       <c r="B404" t="s">
         <v>1041</v>
@@ -7849,15 +7952,15 @@
     </row>
     <row r="405" spans="1:2">
       <c r="A405" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="B405" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="406" spans="1:2">
       <c r="A406" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="B406" t="s">
         <v>1041</v>
@@ -7865,7 +7968,7 @@
     </row>
     <row r="407" spans="1:2">
       <c r="A407" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="B407" t="s">
         <v>1041</v>
@@ -7873,7 +7976,7 @@
     </row>
     <row r="408" spans="1:2">
       <c r="A408" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="B408" t="s">
         <v>1041</v>
@@ -7881,7 +7984,7 @@
     </row>
     <row r="409" spans="1:2">
       <c r="A409" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="B409" t="s">
         <v>1041</v>
@@ -7889,7 +7992,7 @@
     </row>
     <row r="410" spans="1:2">
       <c r="A410" t="s">
-        <v>726</v>
+        <v>730</v>
       </c>
       <c r="B410" t="s">
         <v>1041</v>
@@ -7897,7 +8000,7 @@
     </row>
     <row r="411" spans="1:2">
       <c r="A411" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="B411" t="s">
         <v>1041</v>
@@ -7905,7 +8008,7 @@
     </row>
     <row r="412" spans="1:2">
       <c r="A412" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="B412" t="s">
         <v>1041</v>
@@ -7913,7 +8016,7 @@
     </row>
     <row r="413" spans="1:2">
       <c r="A413" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="B413" t="s">
         <v>1041</v>
@@ -7921,7 +8024,7 @@
     </row>
     <row r="414" spans="1:2">
       <c r="A414" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="B414" t="s">
         <v>1041</v>
@@ -7929,7 +8032,7 @@
     </row>
     <row r="415" spans="1:2">
       <c r="A415" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
       <c r="B415" t="s">
         <v>1041</v>
@@ -7937,7 +8040,7 @@
     </row>
     <row r="416" spans="1:2">
       <c r="A416" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B416" t="s">
         <v>1041</v>
@@ -7945,7 +8048,7 @@
     </row>
     <row r="417" spans="1:2">
       <c r="A417" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
       <c r="B417" t="s">
         <v>1041</v>
@@ -7953,7 +8056,7 @@
     </row>
     <row r="418" spans="1:2">
       <c r="A418" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="B418" t="s">
         <v>1041</v>
@@ -7961,7 +8064,7 @@
     </row>
     <row r="419" spans="1:2">
       <c r="A419" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="B419" t="s">
         <v>1041</v>
@@ -7969,7 +8072,7 @@
     </row>
     <row r="420" spans="1:2">
       <c r="A420" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
       <c r="B420" t="s">
         <v>1041</v>
@@ -7977,7 +8080,7 @@
     </row>
     <row r="421" spans="1:2">
       <c r="A421" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="B421" t="s">
         <v>1041</v>
@@ -7985,7 +8088,7 @@
     </row>
     <row r="422" spans="1:2">
       <c r="A422" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="B422" t="s">
         <v>1041</v>
@@ -7993,7 +8096,7 @@
     </row>
     <row r="423" spans="1:2">
       <c r="A423" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="B423" t="s">
         <v>1041</v>
@@ -8001,7 +8104,7 @@
     </row>
     <row r="424" spans="1:2">
       <c r="A424" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="B424" t="s">
         <v>1041</v>
@@ -8009,7 +8112,7 @@
     </row>
     <row r="425" spans="1:2">
       <c r="A425" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="B425" t="s">
         <v>1041</v>
@@ -8017,7 +8120,7 @@
     </row>
     <row r="426" spans="1:2">
       <c r="A426" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B426" t="s">
         <v>1041</v>
@@ -8025,7 +8128,7 @@
     </row>
     <row r="427" spans="1:2">
       <c r="A427" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="B427" t="s">
         <v>1041</v>
@@ -8033,7 +8136,7 @@
     </row>
     <row r="428" spans="1:2">
       <c r="A428" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="B428" t="s">
         <v>1041</v>
@@ -8041,7 +8144,7 @@
     </row>
     <row r="429" spans="1:2">
       <c r="A429" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B429" t="s">
         <v>1041</v>
@@ -8049,7 +8152,7 @@
     </row>
     <row r="430" spans="1:2">
       <c r="A430" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="B430" t="s">
         <v>1041</v>
@@ -8057,7 +8160,7 @@
     </row>
     <row r="431" spans="1:2">
       <c r="A431" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="B431" t="s">
         <v>1041</v>
@@ -8065,7 +8168,7 @@
     </row>
     <row r="432" spans="1:2">
       <c r="A432" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="B432" t="s">
         <v>1041</v>
@@ -8073,7 +8176,7 @@
     </row>
     <row r="433" spans="1:2">
       <c r="A433" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="B433" t="s">
         <v>1041</v>
@@ -8081,7 +8184,7 @@
     </row>
     <row r="434" spans="1:2">
       <c r="A434" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="B434" t="s">
         <v>1041</v>
@@ -8089,7 +8192,7 @@
     </row>
     <row r="435" spans="1:2">
       <c r="A435" t="s">
-        <v>757</v>
+        <v>762</v>
       </c>
       <c r="B435" t="s">
         <v>1041</v>
@@ -8097,7 +8200,7 @@
     </row>
     <row r="436" spans="1:2">
       <c r="A436" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="B436" t="s">
         <v>1041</v>
@@ -8105,7 +8208,7 @@
     </row>
     <row r="437" spans="1:2">
       <c r="A437" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
       <c r="B437" t="s">
         <v>1041</v>
@@ -8113,7 +8216,7 @@
     </row>
     <row r="438" spans="1:2">
       <c r="A438" t="s">
-        <v>764</v>
+        <v>768</v>
       </c>
       <c r="B438" t="s">
         <v>1041</v>
@@ -8121,7 +8224,7 @@
     </row>
     <row r="439" spans="1:2">
       <c r="A439" t="s">
-        <v>765</v>
+        <v>769</v>
       </c>
       <c r="B439" t="s">
         <v>1041</v>
@@ -8129,7 +8232,7 @@
     </row>
     <row r="440" spans="1:2">
       <c r="A440" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="B440" t="s">
         <v>1041</v>
@@ -8137,7 +8240,7 @@
     </row>
     <row r="441" spans="1:2">
       <c r="A441" t="s">
-        <v>769</v>
+        <v>773</v>
       </c>
       <c r="B441" t="s">
         <v>1041</v>
@@ -8145,7 +8248,7 @@
     </row>
     <row r="442" spans="1:2">
       <c r="A442" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
       <c r="B442" t="s">
         <v>1041</v>
@@ -8153,7 +8256,7 @@
     </row>
     <row r="443" spans="1:2">
       <c r="A443" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="B443" t="s">
         <v>1041</v>
@@ -8161,7 +8264,7 @@
     </row>
     <row r="444" spans="1:2">
       <c r="A444" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="B444" t="s">
         <v>1041</v>
@@ -8169,7 +8272,7 @@
     </row>
     <row r="445" spans="1:2">
       <c r="A445" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="B445" t="s">
         <v>1041</v>
@@ -8177,7 +8280,7 @@
     </row>
     <row r="446" spans="1:2">
       <c r="A446" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="B446" t="s">
         <v>1041</v>
@@ -8185,7 +8288,7 @@
     </row>
     <row r="447" spans="1:2">
       <c r="A447" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="B447" t="s">
         <v>1041</v>
@@ -8193,7 +8296,7 @@
     </row>
     <row r="448" spans="1:2">
       <c r="A448" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B448" t="s">
         <v>1041</v>
@@ -8201,7 +8304,7 @@
     </row>
     <row r="449" spans="1:2">
       <c r="A449" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="B449" t="s">
         <v>1041</v>
@@ -8209,7 +8312,7 @@
     </row>
     <row r="450" spans="1:2">
       <c r="A450" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="B450" t="s">
         <v>1041</v>
@@ -8217,7 +8320,7 @@
     </row>
     <row r="451" spans="1:2">
       <c r="A451" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="B451" t="s">
         <v>1041</v>
@@ -8225,7 +8328,7 @@
     </row>
     <row r="452" spans="1:2">
       <c r="A452" t="s">
-        <v>782</v>
+        <v>787</v>
       </c>
       <c r="B452" t="s">
         <v>1041</v>
@@ -8233,7 +8336,7 @@
     </row>
     <row r="453" spans="1:2">
       <c r="A453" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
       <c r="B453" t="s">
         <v>1041</v>
@@ -8241,7 +8344,7 @@
     </row>
     <row r="454" spans="1:2">
       <c r="A454" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
       <c r="B454" t="s">
         <v>1041</v>
@@ -8249,7 +8352,7 @@
     </row>
     <row r="455" spans="1:2">
       <c r="A455" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="B455" t="s">
         <v>1041</v>
@@ -8257,7 +8360,7 @@
     </row>
     <row r="456" spans="1:2">
       <c r="A456" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="B456" t="s">
         <v>1041</v>
@@ -8265,7 +8368,7 @@
     </row>
     <row r="457" spans="1:2">
       <c r="A457" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B457" t="s">
         <v>1041</v>
@@ -8273,7 +8376,7 @@
     </row>
     <row r="458" spans="1:2">
       <c r="A458" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B458" t="s">
         <v>1041</v>
@@ -8281,7 +8384,7 @@
     </row>
     <row r="459" spans="1:2">
       <c r="A459" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="B459" t="s">
         <v>1041</v>
@@ -8289,7 +8392,7 @@
     </row>
     <row r="460" spans="1:2">
       <c r="A460" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="B460" t="s">
         <v>1041</v>
@@ -8297,7 +8400,7 @@
     </row>
     <row r="461" spans="1:2">
       <c r="A461" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="B461" t="s">
         <v>1041</v>
@@ -8305,7 +8408,7 @@
     </row>
     <row r="462" spans="1:2">
       <c r="A462" t="s">
-        <v>797</v>
+        <v>800</v>
       </c>
       <c r="B462" t="s">
         <v>1041</v>
@@ -8313,7 +8416,7 @@
     </row>
     <row r="463" spans="1:2">
       <c r="A463" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="B463" t="s">
         <v>1041</v>
@@ -8321,7 +8424,7 @@
     </row>
     <row r="464" spans="1:2">
       <c r="A464" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="B464" t="s">
         <v>1041</v>
@@ -8329,7 +8432,7 @@
     </row>
     <row r="465" spans="1:2">
       <c r="A465" t="s">
-        <v>801</v>
+        <v>804</v>
       </c>
       <c r="B465" t="s">
         <v>1041</v>
@@ -8337,7 +8440,7 @@
     </row>
     <row r="466" spans="1:2">
       <c r="A466" t="s">
-        <v>802</v>
+        <v>805</v>
       </c>
       <c r="B466" t="s">
         <v>1041</v>
@@ -8345,7 +8448,7 @@
     </row>
     <row r="467" spans="1:2">
       <c r="A467" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="B467" t="s">
         <v>1041</v>
@@ -8353,7 +8456,7 @@
     </row>
     <row r="468" spans="1:2">
       <c r="A468" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="B468" t="s">
         <v>1041</v>
@@ -8361,7 +8464,7 @@
     </row>
     <row r="469" spans="1:2">
       <c r="A469" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="B469" t="s">
         <v>1041</v>
@@ -8369,7 +8472,7 @@
     </row>
     <row r="470" spans="1:2">
       <c r="A470" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="B470" t="s">
         <v>1041</v>
@@ -8377,7 +8480,7 @@
     </row>
     <row r="471" spans="1:2">
       <c r="A471" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="B471" t="s">
         <v>1041</v>
@@ -8385,7 +8488,7 @@
     </row>
     <row r="472" spans="1:2">
       <c r="A472" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="B472" t="s">
         <v>1041</v>
@@ -8393,7 +8496,7 @@
     </row>
     <row r="473" spans="1:2">
       <c r="A473" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="B473" t="s">
         <v>1041</v>
@@ -8401,7 +8504,7 @@
     </row>
     <row r="474" spans="1:2">
       <c r="A474" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="B474" t="s">
         <v>1041</v>
@@ -8409,7 +8512,7 @@
     </row>
     <row r="475" spans="1:2">
       <c r="A475" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="B475" t="s">
         <v>1041</v>
@@ -8417,7 +8520,7 @@
     </row>
     <row r="476" spans="1:2">
       <c r="A476" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="B476" t="s">
         <v>1041</v>
@@ -8425,7 +8528,7 @@
     </row>
     <row r="477" spans="1:2">
       <c r="A477" t="s">
-        <v>816</v>
+        <v>821</v>
       </c>
       <c r="B477" t="s">
         <v>1041</v>
@@ -8433,7 +8536,7 @@
     </row>
     <row r="478" spans="1:2">
       <c r="A478" t="s">
-        <v>818</v>
+        <v>824</v>
       </c>
       <c r="B478" t="s">
         <v>1041</v>
@@ -8441,7 +8544,7 @@
     </row>
     <row r="479" spans="1:2">
       <c r="A479" t="s">
-        <v>821</v>
+        <v>825</v>
       </c>
       <c r="B479" t="s">
         <v>1041</v>
@@ -8449,7 +8552,7 @@
     </row>
     <row r="480" spans="1:2">
       <c r="A480" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="B480" t="s">
         <v>1041</v>
@@ -8457,7 +8560,7 @@
     </row>
     <row r="481" spans="1:2">
       <c r="A481" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="B481" t="s">
         <v>1041</v>
@@ -8465,7 +8568,7 @@
     </row>
     <row r="482" spans="1:2">
       <c r="A482" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="B482" t="s">
         <v>1041</v>
@@ -8473,7 +8576,7 @@
     </row>
     <row r="483" spans="1:2">
       <c r="A483" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="B483" t="s">
         <v>1041</v>
@@ -8481,7 +8584,7 @@
     </row>
     <row r="484" spans="1:2">
       <c r="A484" t="s">
-        <v>828</v>
+        <v>834</v>
       </c>
       <c r="B484" t="s">
         <v>1041</v>
@@ -8489,7 +8592,7 @@
     </row>
     <row r="485" spans="1:2">
       <c r="A485" t="s">
-        <v>829</v>
+        <v>835</v>
       </c>
       <c r="B485" t="s">
         <v>1041</v>
@@ -8497,7 +8600,7 @@
     </row>
     <row r="486" spans="1:2">
       <c r="A486" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="B486" t="s">
         <v>1041</v>
@@ -8505,7 +8608,7 @@
     </row>
     <row r="487" spans="1:2">
       <c r="A487" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="B487" t="s">
         <v>1041</v>
@@ -8513,7 +8616,7 @@
     </row>
     <row r="488" spans="1:2">
       <c r="A488" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="B488" t="s">
         <v>1041</v>
@@ -8521,7 +8624,7 @@
     </row>
     <row r="489" spans="1:2">
       <c r="A489" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="B489" t="s">
         <v>1041</v>
@@ -8529,7 +8632,7 @@
     </row>
     <row r="490" spans="1:2">
       <c r="A490" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="B490" t="s">
         <v>1041</v>
@@ -8537,7 +8640,7 @@
     </row>
     <row r="491" spans="1:2">
       <c r="A491" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="B491" t="s">
         <v>1041</v>
@@ -8545,7 +8648,7 @@
     </row>
     <row r="492" spans="1:2">
       <c r="A492" t="s">
-        <v>840</v>
+        <v>844</v>
       </c>
       <c r="B492" t="s">
         <v>1041</v>
@@ -8553,7 +8656,7 @@
     </row>
     <row r="493" spans="1:2">
       <c r="A493" t="s">
-        <v>841</v>
+        <v>847</v>
       </c>
       <c r="B493" t="s">
         <v>1041</v>
@@ -8561,7 +8664,7 @@
     </row>
     <row r="494" spans="1:2">
       <c r="A494" t="s">
-        <v>844</v>
+        <v>848</v>
       </c>
       <c r="B494" t="s">
         <v>1041</v>
@@ -8569,7 +8672,7 @@
     </row>
     <row r="495" spans="1:2">
       <c r="A495" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="B495" t="s">
         <v>1041</v>
@@ -8577,7 +8680,7 @@
     </row>
     <row r="496" spans="1:2">
       <c r="A496" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="B496" t="s">
         <v>1041</v>
@@ -8585,7 +8688,7 @@
     </row>
     <row r="497" spans="1:2">
       <c r="A497" t="s">
-        <v>849</v>
+        <v>852</v>
       </c>
       <c r="B497" t="s">
         <v>1041</v>
@@ -8593,7 +8696,7 @@
     </row>
     <row r="498" spans="1:2">
       <c r="A498" t="s">
-        <v>850</v>
+        <v>853</v>
       </c>
       <c r="B498" t="s">
         <v>1041</v>
@@ -8601,7 +8704,7 @@
     </row>
     <row r="499" spans="1:2">
       <c r="A499" t="s">
-        <v>852</v>
+        <v>855</v>
       </c>
       <c r="B499" t="s">
         <v>1041</v>
@@ -8609,7 +8712,7 @@
     </row>
     <row r="500" spans="1:2">
       <c r="A500" t="s">
-        <v>853</v>
+        <v>860</v>
       </c>
       <c r="B500" t="s">
         <v>1041</v>
@@ -8617,7 +8720,7 @@
     </row>
     <row r="501" spans="1:2">
       <c r="A501" t="s">
-        <v>855</v>
+        <v>862</v>
       </c>
       <c r="B501" t="s">
         <v>1041</v>
@@ -8625,7 +8728,7 @@
     </row>
     <row r="502" spans="1:2">
       <c r="A502" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="B502" t="s">
         <v>1041</v>
@@ -8633,7 +8736,7 @@
     </row>
     <row r="503" spans="1:2">
       <c r="A503" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="B503" t="s">
         <v>1041</v>
@@ -8641,7 +8744,7 @@
     </row>
     <row r="504" spans="1:2">
       <c r="A504" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
       <c r="B504" t="s">
         <v>1041</v>
@@ -8649,7 +8752,7 @@
     </row>
     <row r="505" spans="1:2">
       <c r="A505" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="B505" t="s">
         <v>1041</v>
@@ -8657,7 +8760,7 @@
     </row>
     <row r="506" spans="1:2">
       <c r="A506" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="B506" t="s">
         <v>1041</v>
@@ -8665,7 +8768,7 @@
     </row>
     <row r="507" spans="1:2">
       <c r="A507" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="B507" t="s">
         <v>1041</v>
@@ -8673,7 +8776,7 @@
     </row>
     <row r="508" spans="1:2">
       <c r="A508" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="B508" t="s">
         <v>1041</v>
@@ -8681,7 +8784,7 @@
     </row>
     <row r="509" spans="1:2">
       <c r="A509" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="B509" t="s">
         <v>1041</v>
@@ -8689,7 +8792,7 @@
     </row>
     <row r="510" spans="1:2">
       <c r="A510" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="B510" t="s">
         <v>1041</v>
@@ -8697,7 +8800,7 @@
     </row>
     <row r="511" spans="1:2">
       <c r="A511" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="B511" t="s">
         <v>1041</v>
@@ -8705,7 +8808,7 @@
     </row>
     <row r="512" spans="1:2">
       <c r="A512" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="B512" t="s">
         <v>1041</v>
@@ -8713,7 +8816,7 @@
     </row>
     <row r="513" spans="1:2">
       <c r="A513" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="B513" t="s">
         <v>1041</v>
@@ -8721,7 +8824,7 @@
     </row>
     <row r="514" spans="1:2">
       <c r="A514" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="B514" t="s">
         <v>1041</v>
@@ -8729,7 +8832,7 @@
     </row>
     <row r="515" spans="1:2">
       <c r="A515" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="B515" t="s">
         <v>1041</v>
@@ -8737,7 +8840,7 @@
     </row>
     <row r="516" spans="1:2">
       <c r="A516" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="B516" t="s">
         <v>1041</v>
@@ -8745,7 +8848,7 @@
     </row>
     <row r="517" spans="1:2">
       <c r="A517" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="B517" t="s">
         <v>1041</v>
@@ -8753,7 +8856,7 @@
     </row>
     <row r="518" spans="1:2">
       <c r="A518" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B518" t="s">
         <v>1041</v>
@@ -8761,7 +8864,7 @@
     </row>
     <row r="519" spans="1:2">
       <c r="A519" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="B519" t="s">
         <v>1041</v>
@@ -8769,7 +8872,7 @@
     </row>
     <row r="520" spans="1:2">
       <c r="A520" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="B520" t="s">
         <v>1041</v>
@@ -8777,7 +8880,7 @@
     </row>
     <row r="521" spans="1:2">
       <c r="A521" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="B521" t="s">
         <v>1041</v>
@@ -8785,7 +8888,7 @@
     </row>
     <row r="522" spans="1:2">
       <c r="A522" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="B522" t="s">
         <v>1041</v>
@@ -8793,7 +8896,7 @@
     </row>
     <row r="523" spans="1:2">
       <c r="A523" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="B523" t="s">
         <v>1041</v>
@@ -8801,7 +8904,7 @@
     </row>
     <row r="524" spans="1:2">
       <c r="A524" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="B524" t="s">
         <v>1041</v>
@@ -8809,7 +8912,7 @@
     </row>
     <row r="525" spans="1:2">
       <c r="A525" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="B525" t="s">
         <v>1041</v>
@@ -8817,7 +8920,7 @@
     </row>
     <row r="526" spans="1:2">
       <c r="A526" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="B526" t="s">
         <v>1041</v>
@@ -8825,7 +8928,7 @@
     </row>
     <row r="527" spans="1:2">
       <c r="A527" t="s">
-        <v>889</v>
+        <v>893</v>
       </c>
       <c r="B527" t="s">
         <v>1041</v>
@@ -8833,7 +8936,7 @@
     </row>
     <row r="528" spans="1:2">
       <c r="A528" t="s">
-        <v>890</v>
+        <v>894</v>
       </c>
       <c r="B528" t="s">
         <v>1041</v>
@@ -8841,7 +8944,7 @@
     </row>
     <row r="529" spans="1:2">
       <c r="A529" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="B529" t="s">
         <v>1041</v>
@@ -8849,7 +8952,7 @@
     </row>
     <row r="530" spans="1:2">
       <c r="A530" t="s">
-        <v>894</v>
+        <v>900</v>
       </c>
       <c r="B530" t="s">
         <v>1041</v>
@@ -8857,7 +8960,7 @@
     </row>
     <row r="531" spans="1:2">
       <c r="A531" t="s">
-        <v>895</v>
+        <v>903</v>
       </c>
       <c r="B531" t="s">
         <v>1041</v>
@@ -8865,7 +8968,7 @@
     </row>
     <row r="532" spans="1:2">
       <c r="A532" t="s">
-        <v>900</v>
+        <v>904</v>
       </c>
       <c r="B532" t="s">
         <v>1041</v>
@@ -8873,7 +8976,7 @@
     </row>
     <row r="533" spans="1:2">
       <c r="A533" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="B533" t="s">
         <v>1041</v>
@@ -8881,7 +8984,7 @@
     </row>
     <row r="534" spans="1:2">
       <c r="A534" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="B534" t="s">
         <v>1041</v>
@@ -8889,7 +8992,7 @@
     </row>
     <row r="535" spans="1:2">
       <c r="A535" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="B535" t="s">
         <v>1041</v>
@@ -8897,7 +9000,7 @@
     </row>
     <row r="536" spans="1:2">
       <c r="A536" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="B536" t="s">
         <v>1041</v>
@@ -8905,7 +9008,7 @@
     </row>
     <row r="537" spans="1:2">
       <c r="A537" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="B537" t="s">
         <v>1041</v>
@@ -8913,7 +9016,7 @@
     </row>
     <row r="538" spans="1:2">
       <c r="A538" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="B538" t="s">
         <v>1041</v>
@@ -8921,7 +9024,7 @@
     </row>
     <row r="539" spans="1:2">
       <c r="A539" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="B539" t="s">
         <v>1041</v>
@@ -8929,7 +9032,7 @@
     </row>
     <row r="540" spans="1:2">
       <c r="A540" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="B540" t="s">
         <v>1041</v>
@@ -8937,7 +9040,7 @@
     </row>
     <row r="541" spans="1:2">
       <c r="A541" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="B541" t="s">
         <v>1041</v>
@@ -8945,7 +9048,7 @@
     </row>
     <row r="542" spans="1:2">
       <c r="A542" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="B542" t="s">
         <v>1041</v>
@@ -8953,7 +9056,7 @@
     </row>
     <row r="543" spans="1:2">
       <c r="A543" t="s">
-        <v>915</v>
+        <v>920</v>
       </c>
       <c r="B543" t="s">
         <v>1041</v>
@@ -8961,7 +9064,7 @@
     </row>
     <row r="544" spans="1:2">
       <c r="A544" t="s">
-        <v>916</v>
+        <v>921</v>
       </c>
       <c r="B544" t="s">
         <v>1041</v>
@@ -8969,7 +9072,7 @@
     </row>
     <row r="545" spans="1:2">
       <c r="A545" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="B545" t="s">
         <v>1041</v>
@@ -8977,7 +9080,7 @@
     </row>
     <row r="546" spans="1:2">
       <c r="A546" t="s">
-        <v>921</v>
+        <v>925</v>
       </c>
       <c r="B546" t="s">
         <v>1041</v>
@@ -8985,7 +9088,7 @@
     </row>
     <row r="547" spans="1:2">
       <c r="A547" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="B547" t="s">
         <v>1041</v>
@@ -8993,7 +9096,7 @@
     </row>
     <row r="548" spans="1:2">
       <c r="A548" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="B548" t="s">
         <v>1041</v>
@@ -9001,7 +9104,7 @@
     </row>
     <row r="549" spans="1:2">
       <c r="A549" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="B549" t="s">
         <v>1041</v>
@@ -9009,7 +9112,7 @@
     </row>
     <row r="550" spans="1:2">
       <c r="A550" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="B550" t="s">
         <v>1041</v>
@@ -9017,7 +9120,7 @@
     </row>
     <row r="551" spans="1:2">
       <c r="A551" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="B551" t="s">
         <v>1041</v>
@@ -9025,7 +9128,7 @@
     </row>
     <row r="552" spans="1:2">
       <c r="A552" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="B552" t="s">
         <v>1041</v>
@@ -9033,7 +9136,7 @@
     </row>
     <row r="553" spans="1:2">
       <c r="A553" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="B553" t="s">
         <v>1041</v>
@@ -9041,7 +9144,7 @@
     </row>
     <row r="554" spans="1:2">
       <c r="A554" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="B554" t="s">
         <v>1041</v>
@@ -9049,7 +9152,7 @@
     </row>
     <row r="555" spans="1:2">
       <c r="A555" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="B555" t="s">
         <v>1041</v>
@@ -9057,7 +9160,7 @@
     </row>
     <row r="556" spans="1:2">
       <c r="A556" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="B556" t="s">
         <v>1041</v>
@@ -9065,7 +9168,7 @@
     </row>
     <row r="557" spans="1:2">
       <c r="A557" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
       <c r="B557" t="s">
         <v>1041</v>
@@ -9073,7 +9176,7 @@
     </row>
     <row r="558" spans="1:2">
       <c r="A558" t="s">
-        <v>936</v>
+        <v>941</v>
       </c>
       <c r="B558" t="s">
         <v>1041</v>
@@ -9081,7 +9184,7 @@
     </row>
     <row r="559" spans="1:2">
       <c r="A559" t="s">
-        <v>937</v>
+        <v>942</v>
       </c>
       <c r="B559" t="s">
         <v>1041</v>
@@ -9089,7 +9192,7 @@
     </row>
     <row r="560" spans="1:2">
       <c r="A560" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="B560" t="s">
         <v>1041</v>
@@ -9097,7 +9200,7 @@
     </row>
     <row r="561" spans="1:2">
       <c r="A561" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="B561" t="s">
         <v>1041</v>
@@ -9105,7 +9208,7 @@
     </row>
     <row r="562" spans="1:2">
       <c r="A562" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="B562" t="s">
         <v>1041</v>
@@ -9113,7 +9216,7 @@
     </row>
     <row r="563" spans="1:2">
       <c r="A563" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="B563" t="s">
         <v>1041</v>
@@ -9121,7 +9224,7 @@
     </row>
     <row r="564" spans="1:2">
       <c r="A564" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="B564" t="s">
         <v>1041</v>
@@ -9129,7 +9232,7 @@
     </row>
     <row r="565" spans="1:2">
       <c r="A565" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="B565" t="s">
         <v>1041</v>
@@ -9137,7 +9240,7 @@
     </row>
     <row r="566" spans="1:2">
       <c r="A566" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="B566" t="s">
         <v>1041</v>
@@ -9145,7 +9248,7 @@
     </row>
     <row r="567" spans="1:2">
       <c r="A567" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B567" t="s">
         <v>1041</v>
@@ -9153,7 +9256,7 @@
     </row>
     <row r="568" spans="1:2">
       <c r="A568" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B568" t="s">
         <v>1041</v>
@@ -9161,7 +9264,7 @@
     </row>
     <row r="569" spans="1:2">
       <c r="A569" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B569" t="s">
         <v>1041</v>
@@ -9169,7 +9272,7 @@
     </row>
     <row r="570" spans="1:2">
       <c r="A570" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
       <c r="B570" t="s">
         <v>1041</v>
@@ -9177,7 +9280,7 @@
     </row>
     <row r="571" spans="1:2">
       <c r="A571" t="s">
-        <v>953</v>
+        <v>961</v>
       </c>
       <c r="B571" t="s">
         <v>1041</v>
@@ -9185,7 +9288,7 @@
     </row>
     <row r="572" spans="1:2">
       <c r="A572" t="s">
-        <v>955</v>
+        <v>962</v>
       </c>
       <c r="B572" t="s">
         <v>1041</v>
@@ -9193,7 +9296,7 @@
     </row>
     <row r="573" spans="1:2">
       <c r="A573" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="B573" t="s">
         <v>1041</v>
@@ -9201,7 +9304,7 @@
     </row>
     <row r="574" spans="1:2">
       <c r="A574" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
       <c r="B574" t="s">
         <v>1041</v>
@@ -9209,7 +9312,7 @@
     </row>
     <row r="575" spans="1:2">
       <c r="A575" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B575" t="s">
         <v>1041</v>
@@ -9217,7 +9320,7 @@
     </row>
     <row r="576" spans="1:2">
       <c r="A576" t="s">
-        <v>965</v>
+        <v>969</v>
       </c>
       <c r="B576" t="s">
         <v>1041</v>
@@ -9225,7 +9328,7 @@
     </row>
     <row r="577" spans="1:2">
       <c r="A577" t="s">
-        <v>966</v>
+        <v>970</v>
       </c>
       <c r="B577" t="s">
         <v>1041</v>
@@ -9233,7 +9336,7 @@
     </row>
     <row r="578" spans="1:2">
       <c r="A578" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="B578" t="s">
         <v>1041</v>
@@ -9241,7 +9344,7 @@
     </row>
     <row r="579" spans="1:2">
       <c r="A579" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="B579" t="s">
         <v>1041</v>
@@ -9249,7 +9352,7 @@
     </row>
     <row r="580" spans="1:2">
       <c r="A580" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="B580" t="s">
         <v>1041</v>
@@ -9257,7 +9360,7 @@
     </row>
     <row r="581" spans="1:2">
       <c r="A581" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B581" t="s">
         <v>1041</v>
@@ -9265,7 +9368,7 @@
     </row>
     <row r="582" spans="1:2">
       <c r="A582" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B582" t="s">
         <v>1041</v>
@@ -9273,7 +9376,7 @@
     </row>
     <row r="583" spans="1:2">
       <c r="A583" t="s">
-        <v>975</v>
+        <v>979</v>
       </c>
       <c r="B583" t="s">
         <v>1041</v>
@@ -9281,7 +9384,7 @@
     </row>
     <row r="584" spans="1:2">
       <c r="A584" t="s">
-        <v>976</v>
+        <v>981</v>
       </c>
       <c r="B584" t="s">
         <v>1041</v>
@@ -9289,7 +9392,7 @@
     </row>
     <row r="585" spans="1:2">
       <c r="A585" t="s">
-        <v>979</v>
+        <v>983</v>
       </c>
       <c r="B585" t="s">
         <v>1041</v>
@@ -9297,7 +9400,7 @@
     </row>
     <row r="586" spans="1:2">
       <c r="A586" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="B586" t="s">
         <v>1041</v>
@@ -9305,7 +9408,7 @@
     </row>
     <row r="587" spans="1:2">
       <c r="A587" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B587" t="s">
         <v>1041</v>
@@ -9313,7 +9416,7 @@
     </row>
     <row r="588" spans="1:2">
       <c r="A588" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c r="B588" t="s">
         <v>1041</v>
@@ -9321,7 +9424,7 @@
     </row>
     <row r="589" spans="1:2">
       <c r="A589" t="s">
-        <v>985</v>
+        <v>1032</v>
       </c>
       <c r="B589" t="s">
         <v>1041</v>
@@ -9329,7 +9432,7 @@
     </row>
     <row r="590" spans="1:2">
       <c r="A590" t="s">
-        <v>987</v>
+        <v>1034</v>
       </c>
       <c r="B590" t="s">
         <v>1041</v>
@@ -9337,7 +9440,7 @@
     </row>
     <row r="591" spans="1:2">
       <c r="A591" t="s">
-        <v>1032</v>
+        <v>1035</v>
       </c>
       <c r="B591" t="s">
         <v>1041</v>
@@ -9345,7 +9448,7 @@
     </row>
     <row r="592" spans="1:2">
       <c r="A592" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="B592" t="s">
         <v>1041</v>
@@ -9353,7 +9456,7 @@
     </row>
     <row r="593" spans="1:2">
       <c r="A593" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="B593" t="s">
         <v>1041</v>
@@ -9361,7 +9464,7 @@
     </row>
     <row r="594" spans="1:2">
       <c r="A594" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B594" t="s">
         <v>1041</v>
@@ -9369,23 +9472,23 @@
     </row>
     <row r="595" spans="1:2">
       <c r="A595" t="s">
-        <v>1037</v>
+        <v>60</v>
       </c>
       <c r="B595" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="596" spans="1:2">
       <c r="A596" t="s">
-        <v>1038</v>
+        <v>61</v>
       </c>
       <c r="B596" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="597" spans="1:2">
       <c r="A597" t="s">
-        <v>60</v>
+        <v>97</v>
       </c>
       <c r="B597" t="s">
         <v>1039</v>
@@ -9393,7 +9496,7 @@
     </row>
     <row r="598" spans="1:2">
       <c r="A598" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
       <c r="B598" t="s">
         <v>1039</v>
@@ -9401,7 +9504,7 @@
     </row>
     <row r="599" spans="1:2">
       <c r="A599" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
       <c r="B599" t="s">
         <v>1039</v>
@@ -9409,7 +9512,7 @@
     </row>
     <row r="600" spans="1:2">
       <c r="A600" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="B600" t="s">
         <v>1039</v>
@@ -9417,7 +9520,7 @@
     </row>
     <row r="601" spans="1:2">
       <c r="A601" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="B601" t="s">
         <v>1039</v>
@@ -9425,7 +9528,7 @@
     </row>
     <row r="602" spans="1:2">
       <c r="A602" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B602" t="s">
         <v>1039</v>
@@ -9433,7 +9536,7 @@
     </row>
     <row r="603" spans="1:2">
       <c r="A603" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="B603" t="s">
         <v>1039</v>
@@ -9441,7 +9544,7 @@
     </row>
     <row r="604" spans="1:2">
       <c r="A604" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="B604" t="s">
         <v>1039</v>
@@ -9449,7 +9552,7 @@
     </row>
     <row r="605" spans="1:2">
       <c r="A605" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B605" t="s">
         <v>1039</v>
@@ -9457,7 +9560,7 @@
     </row>
     <row r="606" spans="1:2">
       <c r="A606" t="s">
-        <v>173</v>
+        <v>269</v>
       </c>
       <c r="B606" t="s">
         <v>1039</v>
@@ -9465,7 +9568,7 @@
     </row>
     <row r="607" spans="1:2">
       <c r="A607" t="s">
-        <v>184</v>
+        <v>460</v>
       </c>
       <c r="B607" t="s">
         <v>1039</v>
@@ -9473,7 +9576,7 @@
     </row>
     <row r="608" spans="1:2">
       <c r="A608" t="s">
-        <v>269</v>
+        <v>481</v>
       </c>
       <c r="B608" t="s">
         <v>1039</v>
@@ -9481,7 +9584,7 @@
     </row>
     <row r="609" spans="1:2">
       <c r="A609" t="s">
-        <v>460</v>
+        <v>504</v>
       </c>
       <c r="B609" t="s">
         <v>1039</v>
@@ -9489,7 +9592,7 @@
     </row>
     <row r="610" spans="1:2">
       <c r="A610" t="s">
-        <v>481</v>
+        <v>517</v>
       </c>
       <c r="B610" t="s">
         <v>1039</v>
@@ -9497,7 +9600,7 @@
     </row>
     <row r="611" spans="1:2">
       <c r="A611" t="s">
-        <v>504</v>
+        <v>583</v>
       </c>
       <c r="B611" t="s">
         <v>1039</v>
@@ -9505,7 +9608,7 @@
     </row>
     <row r="612" spans="1:2">
       <c r="A612" t="s">
-        <v>517</v>
+        <v>584</v>
       </c>
       <c r="B612" t="s">
         <v>1039</v>
@@ -9513,7 +9616,7 @@
     </row>
     <row r="613" spans="1:2">
       <c r="A613" t="s">
-        <v>583</v>
+        <v>601</v>
       </c>
       <c r="B613" t="s">
         <v>1039</v>
@@ -9521,7 +9624,7 @@
     </row>
     <row r="614" spans="1:2">
       <c r="A614" t="s">
-        <v>584</v>
+        <v>614</v>
       </c>
       <c r="B614" t="s">
         <v>1039</v>
@@ -9529,7 +9632,7 @@
     </row>
     <row r="615" spans="1:2">
       <c r="A615" t="s">
-        <v>601</v>
+        <v>656</v>
       </c>
       <c r="B615" t="s">
         <v>1039</v>
@@ -9537,7 +9640,7 @@
     </row>
     <row r="616" spans="1:2">
       <c r="A616" t="s">
-        <v>614</v>
+        <v>674</v>
       </c>
       <c r="B616" t="s">
         <v>1039</v>
@@ -9545,7 +9648,7 @@
     </row>
     <row r="617" spans="1:2">
       <c r="A617" t="s">
-        <v>656</v>
+        <v>675</v>
       </c>
       <c r="B617" t="s">
         <v>1039</v>
@@ -9553,7 +9656,7 @@
     </row>
     <row r="618" spans="1:2">
       <c r="A618" t="s">
-        <v>674</v>
+        <v>676</v>
       </c>
       <c r="B618" t="s">
         <v>1039</v>
@@ -9561,7 +9664,7 @@
     </row>
     <row r="619" spans="1:2">
       <c r="A619" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="B619" t="s">
         <v>1039</v>
@@ -9569,7 +9672,7 @@
     </row>
     <row r="620" spans="1:2">
       <c r="A620" t="s">
-        <v>676</v>
+        <v>681</v>
       </c>
       <c r="B620" t="s">
         <v>1039</v>
@@ -9577,7 +9680,7 @@
     </row>
     <row r="621" spans="1:2">
       <c r="A621" t="s">
-        <v>679</v>
+        <v>692</v>
       </c>
       <c r="B621" t="s">
         <v>1039</v>
@@ -9585,7 +9688,7 @@
     </row>
     <row r="622" spans="1:2">
       <c r="A622" t="s">
-        <v>681</v>
+        <v>708</v>
       </c>
       <c r="B622" t="s">
         <v>1039</v>
@@ -9593,7 +9696,7 @@
     </row>
     <row r="623" spans="1:2">
       <c r="A623" t="s">
-        <v>692</v>
+        <v>719</v>
       </c>
       <c r="B623" t="s">
         <v>1039</v>
@@ -9601,33 +9704,18 @@
     </row>
     <row r="624" spans="1:2">
       <c r="A624" t="s">
-        <v>708</v>
+        <v>742</v>
       </c>
       <c r="B624" t="s">
         <v>1039</v>
       </c>
     </row>
-    <row r="625" spans="1:2">
-      <c r="A625" t="s">
-        <v>719</v>
-      </c>
-      <c r="B625" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="626" spans="1:2">
-      <c r="A626" t="s">
-        <v>742</v>
-      </c>
-      <c r="B626" t="s">
-        <v>1039</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A626">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="A2:A624">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>